<commit_message>
Re-added the check on the real database for sample uniqueness and existence of researcher.
The test database appears to be populated. I was trying to figure out how to initialize it as empty, but could not figure it out.  However, I did confirm that the tests are not leaving the database modified.

Files checked in: DataRepo/example_data/data_submission_animal_sample_table.xlsx DataRepo/utils.py DataRepo/views.py
[skip ci]
</commit_message>
<xml_diff>
--- a/DataRepo/example_data/data_submission_animal_sample_table.xlsx
+++ b/DataRepo/example_data/data_submission_animal_sample_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/GoogleDrivePU/PROJECT/TRACEBASE/REPO/TraceBase/DataRepo/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DAC7D57-4512-4342-BC5C-1CAA4347BA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E3D6B5-A08E-8544-8E73-68BBA96C2B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9940" yWindow="1040" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Animals" sheetId="1" r:id="rId1"/>
@@ -586,9 +586,6 @@
     <t>M1_15_ears</t>
   </si>
   <si>
-    <t>Matt McBride</t>
-  </si>
-  <si>
     <t>serum</t>
   </si>
   <si>
@@ -933,6 +930,9 @@
   <si>
     <t>Mice on serine and glycine free AA purified diet for 3 weeks</t>
   </si>
+  <si>
+    <t>Anonymous</t>
+  </si>
 </sst>
 </file>
 
@@ -1228,7 +1228,7 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J2" sqref="J2:J3"/>
     </sheetView>
@@ -1495,7 +1495,7 @@
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -1530,7 +1530,7 @@
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
@@ -1600,7 +1600,7 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -1670,7 +1670,7 @@
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
@@ -1717,9 +1717,9 @@
   </sheetPr>
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C192" sqref="C192"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1783,13 +1783,13 @@
         <v>44077</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>17</v>
@@ -1813,13 +1813,13 @@
         <v>44077</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="E3" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>17</v>
@@ -1843,13 +1843,13 @@
         <v>44077</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>17</v>
@@ -1873,13 +1873,13 @@
         <v>44077</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>17</v>
@@ -1903,13 +1903,13 @@
         <v>44077</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>17</v>
@@ -1933,13 +1933,13 @@
         <v>44077</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>17</v>
@@ -1963,13 +1963,13 @@
         <v>44077</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>17</v>
@@ -1993,13 +1993,13 @@
         <v>44077</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>17</v>
@@ -2023,13 +2023,13 @@
         <v>44077</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>17</v>
@@ -2053,13 +2053,13 @@
         <v>44077</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>17</v>
@@ -2083,13 +2083,13 @@
         <v>44077</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>17</v>
@@ -2113,13 +2113,13 @@
         <v>44077</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>17</v>
@@ -2143,13 +2143,13 @@
         <v>44077</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>17</v>
@@ -2173,13 +2173,13 @@
         <v>44077</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>17</v>
@@ -2203,13 +2203,13 @@
         <v>44077</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>17</v>
@@ -2233,13 +2233,13 @@
         <v>44077</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>17</v>
@@ -2257,19 +2257,19 @@
     </row>
     <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18" s="12">
         <v>44077</v>
       </c>
       <c r="C18" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>25</v>
@@ -2287,19 +2287,19 @@
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B19" s="12">
         <v>44077</v>
       </c>
       <c r="C19" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="E19" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>25</v>
@@ -2317,19 +2317,19 @@
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" s="12">
         <v>44077</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>25</v>
@@ -2347,19 +2347,19 @@
     </row>
     <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B21" s="12">
         <v>44077</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>25</v>
@@ -2377,19 +2377,19 @@
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B22" s="12">
         <v>44077</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>25</v>
@@ -2407,19 +2407,19 @@
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" s="12">
         <v>44077</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>25</v>
@@ -2437,19 +2437,19 @@
     </row>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B24" s="12">
         <v>44077</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>25</v>
@@ -2467,19 +2467,19 @@
     </row>
     <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B25" s="12">
         <v>44077</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>25</v>
@@ -2497,19 +2497,19 @@
     </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B26" s="12">
         <v>44077</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>25</v>
@@ -2527,19 +2527,19 @@
     </row>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" s="12">
         <v>44077</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>25</v>
@@ -2557,19 +2557,19 @@
     </row>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28" s="12">
         <v>44077</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>25</v>
@@ -2587,19 +2587,19 @@
     </row>
     <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B29" s="12">
         <v>44077</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>25</v>
@@ -2617,19 +2617,19 @@
     </row>
     <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="12">
         <v>44077</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>25</v>
@@ -2647,19 +2647,19 @@
     </row>
     <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" s="12">
         <v>44077</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>25</v>
@@ -2677,19 +2677,19 @@
     </row>
     <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B32" s="12">
         <v>44077</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>25</v>
@@ -2707,19 +2707,19 @@
     </row>
     <row r="33" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B33" s="12">
         <v>44077</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>25</v>
@@ -2737,19 +2737,19 @@
     </row>
     <row r="34" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B34" s="12">
         <v>44077</v>
       </c>
       <c r="C34" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="E34" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>27</v>
@@ -2767,19 +2767,19 @@
     </row>
     <row r="35" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35" s="12">
         <v>44077</v>
       </c>
       <c r="C35" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="E35" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>27</v>
@@ -2797,19 +2797,19 @@
     </row>
     <row r="36" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B36" s="12">
         <v>44077</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>27</v>
@@ -2827,19 +2827,19 @@
     </row>
     <row r="37" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B37" s="12">
         <v>44077</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>27</v>
@@ -2857,19 +2857,19 @@
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B38" s="12">
         <v>44077</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>27</v>
@@ -2887,19 +2887,19 @@
     </row>
     <row r="39" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B39" s="12">
         <v>44077</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>27</v>
@@ -2917,19 +2917,19 @@
     </row>
     <row r="40" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B40" s="12">
         <v>44077</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>27</v>
@@ -2947,19 +2947,19 @@
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" s="12">
         <v>44077</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>27</v>
@@ -2977,19 +2977,19 @@
     </row>
     <row r="42" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B42" s="12">
         <v>44077</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>27</v>
@@ -3007,19 +3007,19 @@
     </row>
     <row r="43" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B43" s="12">
         <v>44077</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>27</v>
@@ -3037,19 +3037,19 @@
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44" s="12">
         <v>44077</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>27</v>
@@ -3067,19 +3067,19 @@
     </row>
     <row r="45" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B45" s="12">
         <v>44077</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>27</v>
@@ -3097,19 +3097,19 @@
     </row>
     <row r="46" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B46" s="12">
         <v>44077</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>27</v>
@@ -3127,19 +3127,19 @@
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B47" s="12">
         <v>44077</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>27</v>
@@ -3157,19 +3157,19 @@
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B48" s="12">
         <v>44077</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>27</v>
@@ -3187,19 +3187,19 @@
     </row>
     <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B49" s="12">
         <v>44077</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>27</v>
@@ -3217,19 +3217,19 @@
     </row>
     <row r="50" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B50" s="12">
         <v>44077</v>
       </c>
       <c r="C50" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="E50" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>28</v>
@@ -3247,19 +3247,19 @@
     </row>
     <row r="51" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B51" s="12">
         <v>44077</v>
       </c>
       <c r="C51" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D51" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="E51" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>28</v>
@@ -3277,19 +3277,19 @@
     </row>
     <row r="52" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B52" s="12">
         <v>44077</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>28</v>
@@ -3307,19 +3307,19 @@
     </row>
     <row r="53" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B53" s="12">
         <v>44077</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>28</v>
@@ -3337,19 +3337,19 @@
     </row>
     <row r="54" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B54" s="12">
         <v>44077</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>28</v>
@@ -3367,19 +3367,19 @@
     </row>
     <row r="55" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B55" s="12">
         <v>44077</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>28</v>
@@ -3397,19 +3397,19 @@
     </row>
     <row r="56" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B56" s="12">
         <v>44077</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>28</v>
@@ -3427,19 +3427,19 @@
     </row>
     <row r="57" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B57" s="12">
         <v>44077</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>28</v>
@@ -3457,19 +3457,19 @@
     </row>
     <row r="58" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B58" s="12">
         <v>44077</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>28</v>
@@ -3487,19 +3487,19 @@
     </row>
     <row r="59" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B59" s="12">
         <v>44077</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>28</v>
@@ -3517,19 +3517,19 @@
     </row>
     <row r="60" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B60" s="12">
         <v>44077</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>28</v>
@@ -3547,19 +3547,19 @@
     </row>
     <row r="61" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B61" s="12">
         <v>44077</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>28</v>
@@ -3577,19 +3577,19 @@
     </row>
     <row r="62" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B62" s="12">
         <v>44077</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>28</v>
@@ -3607,19 +3607,19 @@
     </row>
     <row r="63" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B63" s="12">
         <v>44077</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>28</v>
@@ -3637,19 +3637,19 @@
     </row>
     <row r="64" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B64" s="12">
         <v>44077</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>28</v>
@@ -3667,19 +3667,19 @@
     </row>
     <row r="65" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B65" s="12">
         <v>44077</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>28</v>
@@ -3697,19 +3697,19 @@
     </row>
     <row r="66" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A66" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B66" s="12">
         <v>44077</v>
       </c>
       <c r="C66" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D66" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="E66" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>29</v>
@@ -3727,19 +3727,19 @@
     </row>
     <row r="67" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B67" s="12">
         <v>44077</v>
       </c>
       <c r="C67" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D67" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D67" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="E67" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>29</v>
@@ -3757,19 +3757,19 @@
     </row>
     <row r="68" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B68" s="12">
         <v>44077</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>29</v>
@@ -3787,19 +3787,19 @@
     </row>
     <row r="69" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A69" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B69" s="12">
         <v>44077</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>29</v>
@@ -3817,19 +3817,19 @@
     </row>
     <row r="70" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A70" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B70" s="12">
         <v>44077</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>29</v>
@@ -3847,19 +3847,19 @@
     </row>
     <row r="71" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B71" s="12">
         <v>44077</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>29</v>
@@ -3877,19 +3877,19 @@
     </row>
     <row r="72" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B72" s="12">
         <v>44077</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>29</v>
@@ -3907,19 +3907,19 @@
     </row>
     <row r="73" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B73" s="12">
         <v>44077</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>29</v>
@@ -3937,19 +3937,19 @@
     </row>
     <row r="74" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B74" s="12">
         <v>44077</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>29</v>
@@ -3967,19 +3967,19 @@
     </row>
     <row r="75" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A75" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B75" s="12">
         <v>44077</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>29</v>
@@ -3997,19 +3997,19 @@
     </row>
     <row r="76" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B76" s="12">
         <v>44077</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>29</v>
@@ -4027,19 +4027,19 @@
     </row>
     <row r="77" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B77" s="12">
         <v>44077</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>29</v>
@@ -4057,19 +4057,19 @@
     </row>
     <row r="78" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B78" s="12">
         <v>44077</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>29</v>
@@ -4087,19 +4087,19 @@
     </row>
     <row r="79" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A79" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B79" s="12">
         <v>44077</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>29</v>
@@ -4117,19 +4117,19 @@
     </row>
     <row r="80" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B80" s="12">
         <v>44077</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>29</v>
@@ -4147,19 +4147,19 @@
     </row>
     <row r="81" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B81" s="12">
         <v>44077</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F81" s="6" t="s">
         <v>29</v>
@@ -4177,19 +4177,19 @@
     </row>
     <row r="82" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B82" s="12">
         <v>44077</v>
       </c>
       <c r="C82" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D82" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D82" s="6" t="s">
+      <c r="E82" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>30</v>
@@ -4207,19 +4207,19 @@
     </row>
     <row r="83" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B83" s="12">
         <v>44077</v>
       </c>
       <c r="C83" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D83" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D83" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="E83" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F83" s="6" t="s">
         <v>30</v>
@@ -4237,19 +4237,19 @@
     </row>
     <row r="84" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B84" s="12">
         <v>44077</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>30</v>
@@ -4267,19 +4267,19 @@
     </row>
     <row r="85" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B85" s="12">
         <v>44077</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>30</v>
@@ -4297,19 +4297,19 @@
     </row>
     <row r="86" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B86" s="12">
         <v>44077</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>30</v>
@@ -4327,19 +4327,19 @@
     </row>
     <row r="87" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B87" s="12">
         <v>44077</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F87" s="6" t="s">
         <v>30</v>
@@ -4357,19 +4357,19 @@
     </row>
     <row r="88" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B88" s="12">
         <v>44077</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F88" s="6" t="s">
         <v>30</v>
@@ -4387,19 +4387,19 @@
     </row>
     <row r="89" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B89" s="12">
         <v>44077</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>30</v>
@@ -4417,19 +4417,19 @@
     </row>
     <row r="90" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B90" s="12">
         <v>44077</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>30</v>
@@ -4447,19 +4447,19 @@
     </row>
     <row r="91" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B91" s="12">
         <v>44077</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F91" s="6" t="s">
         <v>30</v>
@@ -4477,19 +4477,19 @@
     </row>
     <row r="92" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B92" s="12">
         <v>44077</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>30</v>
@@ -4507,19 +4507,19 @@
     </row>
     <row r="93" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B93" s="12">
         <v>44077</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F93" s="6" t="s">
         <v>30</v>
@@ -4537,19 +4537,19 @@
     </row>
     <row r="94" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B94" s="12">
         <v>44077</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F94" s="6" t="s">
         <v>30</v>
@@ -4567,19 +4567,19 @@
     </row>
     <row r="95" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B95" s="12">
         <v>44077</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F95" s="6" t="s">
         <v>30</v>
@@ -4597,19 +4597,19 @@
     </row>
     <row r="96" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B96" s="12">
         <v>44077</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F96" s="6" t="s">
         <v>30</v>
@@ -4627,19 +4627,19 @@
     </row>
     <row r="97" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B97" s="12">
         <v>44077</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F97" s="6" t="s">
         <v>30</v>
@@ -4657,22 +4657,22 @@
     </row>
     <row r="98" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B98" s="12">
         <v>44041</v>
       </c>
       <c r="C98" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D98" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D98" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="E98" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G98" s="6"/>
       <c r="H98" s="6"/>
@@ -4687,22 +4687,22 @@
     </row>
     <row r="99" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B99" s="12">
         <v>44041</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F99" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G99" s="6"/>
       <c r="H99" s="6"/>
@@ -4723,16 +4723,16 @@
         <v>44041</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G100" s="6"/>
       <c r="H100" s="6"/>
@@ -4753,16 +4753,16 @@
         <v>44041</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G101" s="6"/>
       <c r="H101" s="6"/>
@@ -4783,16 +4783,16 @@
         <v>44041</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F102" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G102" s="6"/>
       <c r="H102" s="6"/>
@@ -4813,16 +4813,16 @@
         <v>44041</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G103" s="6"/>
       <c r="H103" s="6"/>
@@ -4843,16 +4843,16 @@
         <v>44041</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F104" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G104" s="6"/>
       <c r="H104" s="6"/>
@@ -4873,16 +4873,16 @@
         <v>44041</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G105" s="6"/>
       <c r="H105" s="6"/>
@@ -4903,16 +4903,16 @@
         <v>44041</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F106" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G106" s="6"/>
       <c r="H106" s="6"/>
@@ -4933,16 +4933,16 @@
         <v>44041</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F107" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G107" s="6"/>
       <c r="H107" s="6"/>
@@ -4963,16 +4963,16 @@
         <v>44041</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F108" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G108" s="6"/>
       <c r="H108" s="6"/>
@@ -4993,16 +4993,16 @@
         <v>44041</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F109" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G109" s="6"/>
       <c r="H109" s="6"/>
@@ -5023,16 +5023,16 @@
         <v>44041</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F110" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G110" s="6"/>
       <c r="H110" s="6"/>
@@ -5053,16 +5053,16 @@
         <v>44041</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F111" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G111" s="6"/>
       <c r="H111" s="6"/>
@@ -5083,16 +5083,16 @@
         <v>44041</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G112" s="6"/>
       <c r="H112" s="6"/>
@@ -5107,22 +5107,22 @@
     </row>
     <row r="113" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A113" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B113" s="12">
         <v>44041</v>
       </c>
       <c r="C113" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D113" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D113" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="E113" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F113" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G113" s="6"/>
       <c r="H113" s="6"/>
@@ -5137,22 +5137,22 @@
     </row>
     <row r="114" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A114" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B114" s="12">
         <v>44041</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G114" s="6"/>
       <c r="H114" s="6"/>
@@ -5167,22 +5167,22 @@
     </row>
     <row r="115" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A115" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B115" s="12">
         <v>44041</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G115" s="6"/>
       <c r="H115" s="6"/>
@@ -5197,22 +5197,22 @@
     </row>
     <row r="116" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A116" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B116" s="12">
         <v>44041</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F116" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G116" s="6"/>
       <c r="H116" s="6"/>
@@ -5227,22 +5227,22 @@
     </row>
     <row r="117" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A117" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B117" s="12">
         <v>44041</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G117" s="6"/>
       <c r="H117" s="6"/>
@@ -5257,22 +5257,22 @@
     </row>
     <row r="118" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A118" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B118" s="12">
         <v>44041</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G118" s="6"/>
       <c r="H118" s="6"/>
@@ -5287,22 +5287,22 @@
     </row>
     <row r="119" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A119" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B119" s="12">
         <v>44041</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G119" s="6"/>
       <c r="H119" s="6"/>
@@ -5317,22 +5317,22 @@
     </row>
     <row r="120" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A120" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B120" s="12">
         <v>44041</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G120" s="6"/>
       <c r="H120" s="6"/>
@@ -5347,22 +5347,22 @@
     </row>
     <row r="121" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A121" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B121" s="12">
         <v>44041</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G121" s="6"/>
       <c r="H121" s="6"/>
@@ -5377,22 +5377,22 @@
     </row>
     <row r="122" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B122" s="12">
         <v>44041</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G122" s="6"/>
       <c r="H122" s="6"/>
@@ -5407,22 +5407,22 @@
     </row>
     <row r="123" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A123" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B123" s="12">
         <v>44041</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E123" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F123" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G123" s="6"/>
       <c r="H123" s="6"/>
@@ -5437,22 +5437,22 @@
     </row>
     <row r="124" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A124" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B124" s="12">
         <v>44041</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G124" s="6"/>
       <c r="H124" s="6"/>
@@ -5467,22 +5467,22 @@
     </row>
     <row r="125" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A125" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B125" s="12">
         <v>44041</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F125" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G125" s="6"/>
       <c r="H125" s="6"/>
@@ -5497,22 +5497,22 @@
     </row>
     <row r="126" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A126" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B126" s="12">
         <v>44041</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F126" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G126" s="6"/>
       <c r="H126" s="6"/>
@@ -5527,22 +5527,22 @@
     </row>
     <row r="127" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A127" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B127" s="12">
         <v>44041</v>
       </c>
       <c r="C127" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D127" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D127" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="E127" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F127" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G127" s="6"/>
       <c r="H127" s="6"/>
@@ -5557,22 +5557,22 @@
     </row>
     <row r="128" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A128" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B128" s="12">
         <v>44041</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F128" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G128" s="6"/>
       <c r="H128" s="6"/>
@@ -5587,22 +5587,22 @@
     </row>
     <row r="129" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A129" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B129" s="12">
         <v>44041</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F129" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G129" s="6"/>
       <c r="H129" s="6"/>
@@ -5617,22 +5617,22 @@
     </row>
     <row r="130" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A130" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B130" s="12">
         <v>44041</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F130" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G130" s="6"/>
       <c r="H130" s="6"/>
@@ -5647,22 +5647,22 @@
     </row>
     <row r="131" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A131" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B131" s="12">
         <v>44041</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F131" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G131" s="6"/>
       <c r="H131" s="6"/>
@@ -5677,22 +5677,22 @@
     </row>
     <row r="132" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A132" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B132" s="12">
         <v>44041</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F132" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G132" s="6"/>
       <c r="H132" s="6"/>
@@ -5707,22 +5707,22 @@
     </row>
     <row r="133" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A133" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B133" s="12">
         <v>44041</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F133" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G133" s="6"/>
       <c r="H133" s="6"/>
@@ -5737,22 +5737,22 @@
     </row>
     <row r="134" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A134" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B134" s="12">
         <v>44041</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E134" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F134" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G134" s="6"/>
       <c r="H134" s="6"/>
@@ -5767,22 +5767,22 @@
     </row>
     <row r="135" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A135" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B135" s="12">
         <v>44041</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E135" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F135" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G135" s="6"/>
       <c r="H135" s="6"/>
@@ -5797,22 +5797,22 @@
     </row>
     <row r="136" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A136" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B136" s="12">
         <v>44041</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F136" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G136" s="6"/>
       <c r="H136" s="6"/>
@@ -5827,22 +5827,22 @@
     </row>
     <row r="137" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A137" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B137" s="12">
         <v>44041</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F137" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G137" s="6"/>
       <c r="H137" s="6"/>
@@ -5857,22 +5857,22 @@
     </row>
     <row r="138" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A138" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B138" s="12">
         <v>44041</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D138" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F138" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G138" s="6"/>
       <c r="H138" s="6"/>
@@ -5887,22 +5887,22 @@
     </row>
     <row r="139" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A139" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B139" s="12">
         <v>44041</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F139" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G139" s="6"/>
       <c r="H139" s="6"/>
@@ -5917,22 +5917,22 @@
     </row>
     <row r="140" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A140" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B140" s="12">
         <v>44041</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F140" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G140" s="6"/>
       <c r="H140" s="6"/>
@@ -5947,22 +5947,22 @@
     </row>
     <row r="141" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A141" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B141" s="12">
         <v>44055</v>
       </c>
       <c r="C141" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D141" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D141" s="6" t="s">
+      <c r="E141" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E141" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="F141" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G141" s="6"/>
       <c r="H141" s="6"/>
@@ -5977,22 +5977,22 @@
     </row>
     <row r="142" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A142" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B142" s="12">
         <v>44055</v>
       </c>
       <c r="C142" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D142" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D142" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="E142" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F142" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G142" s="6"/>
       <c r="H142" s="6"/>
@@ -6007,22 +6007,22 @@
     </row>
     <row r="143" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A143" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B143" s="12">
         <v>44055</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F143" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G143" s="6"/>
       <c r="H143" s="6"/>
@@ -6043,16 +6043,16 @@
         <v>44055</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E144" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F144" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G144" s="6"/>
       <c r="H144" s="6"/>
@@ -6073,16 +6073,16 @@
         <v>44055</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E145" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F145" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G145" s="6"/>
       <c r="H145" s="6"/>
@@ -6103,16 +6103,16 @@
         <v>44055</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E146" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F146" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G146" s="6"/>
       <c r="H146" s="6"/>
@@ -6133,16 +6133,16 @@
         <v>44055</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F147" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G147" s="6"/>
       <c r="H147" s="6"/>
@@ -6163,16 +6163,16 @@
         <v>44055</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E148" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F148" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G148" s="6"/>
       <c r="H148" s="6"/>
@@ -6193,16 +6193,16 @@
         <v>44055</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E149" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F149" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G149" s="6"/>
       <c r="H149" s="6"/>
@@ -6223,16 +6223,16 @@
         <v>44055</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E150" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F150" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G150" s="6"/>
       <c r="H150" s="6"/>
@@ -6253,16 +6253,16 @@
         <v>44055</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E151" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F151" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G151" s="6"/>
       <c r="H151" s="6"/>
@@ -6283,16 +6283,16 @@
         <v>44055</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E152" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F152" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G152" s="6"/>
       <c r="H152" s="6"/>
@@ -6313,16 +6313,16 @@
         <v>44055</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E153" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F153" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G153" s="6"/>
       <c r="H153" s="6"/>
@@ -6343,16 +6343,16 @@
         <v>44055</v>
       </c>
       <c r="C154" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E154" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F154" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G154" s="6"/>
       <c r="H154" s="6"/>
@@ -6373,16 +6373,16 @@
         <v>44055</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F155" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G155" s="6"/>
       <c r="H155" s="6"/>
@@ -6403,16 +6403,16 @@
         <v>44055</v>
       </c>
       <c r="C156" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E156" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F156" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G156" s="6"/>
       <c r="H156" s="6"/>
@@ -6427,22 +6427,22 @@
     </row>
     <row r="157" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A157" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B157" s="12">
         <v>44055</v>
       </c>
       <c r="C157" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D157" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D157" s="6" t="s">
+      <c r="E157" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E157" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="F157" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G157" s="6"/>
       <c r="H157" s="6"/>
@@ -6457,22 +6457,22 @@
     </row>
     <row r="158" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A158" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B158" s="12">
         <v>44055</v>
       </c>
       <c r="C158" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D158" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D158" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="E158" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F158" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G158" s="6"/>
       <c r="H158" s="6"/>
@@ -6487,22 +6487,22 @@
     </row>
     <row r="159" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A159" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B159" s="12">
         <v>44055</v>
       </c>
       <c r="C159" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E159" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F159" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G159" s="6"/>
       <c r="H159" s="6"/>
@@ -6517,22 +6517,22 @@
     </row>
     <row r="160" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A160" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B160" s="12">
         <v>44055</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D160" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E160" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F160" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G160" s="6"/>
       <c r="H160" s="6"/>
@@ -6547,22 +6547,22 @@
     </row>
     <row r="161" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A161" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B161" s="12">
         <v>44055</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E161" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F161" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G161" s="6"/>
       <c r="H161" s="6"/>
@@ -6577,22 +6577,22 @@
     </row>
     <row r="162" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A162" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B162" s="12">
         <v>44055</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D162" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E162" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F162" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G162" s="6"/>
       <c r="H162" s="6"/>
@@ -6607,22 +6607,22 @@
     </row>
     <row r="163" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A163" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B163" s="12">
         <v>44055</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D163" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E163" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F163" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G163" s="6"/>
       <c r="H163" s="6"/>
@@ -6637,22 +6637,22 @@
     </row>
     <row r="164" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A164" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B164" s="12">
         <v>44055</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E164" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F164" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G164" s="6"/>
       <c r="H164" s="6"/>
@@ -6667,22 +6667,22 @@
     </row>
     <row r="165" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A165" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B165" s="12">
         <v>44055</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D165" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E165" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F165" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G165" s="6"/>
       <c r="H165" s="6"/>
@@ -6697,22 +6697,22 @@
     </row>
     <row r="166" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A166" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B166" s="12">
         <v>44055</v>
       </c>
       <c r="C166" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D166" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E166" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F166" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G166" s="6"/>
       <c r="H166" s="6"/>
@@ -6727,22 +6727,22 @@
     </row>
     <row r="167" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A167" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B167" s="12">
         <v>44055</v>
       </c>
       <c r="C167" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D167" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E167" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F167" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G167" s="6"/>
       <c r="H167" s="6"/>
@@ -6757,22 +6757,22 @@
     </row>
     <row r="168" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A168" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B168" s="12">
         <v>44055</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D168" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E168" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F168" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G168" s="6"/>
       <c r="H168" s="6"/>
@@ -6787,22 +6787,22 @@
     </row>
     <row r="169" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A169" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B169" s="12">
         <v>44055</v>
       </c>
       <c r="C169" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D169" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F169" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G169" s="6"/>
       <c r="H169" s="6"/>
@@ -6817,22 +6817,22 @@
     </row>
     <row r="170" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A170" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B170" s="12">
         <v>44055</v>
       </c>
       <c r="C170" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E170" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F170" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G170" s="6"/>
       <c r="H170" s="6"/>
@@ -6847,22 +6847,22 @@
     </row>
     <row r="171" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A171" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B171" s="12">
         <v>44055</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E171" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F171" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G171" s="6"/>
       <c r="H171" s="6"/>
@@ -6877,22 +6877,22 @@
     </row>
     <row r="172" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A172" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B172" s="12">
         <v>44055</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D172" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E172" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F172" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G172" s="6"/>
       <c r="H172" s="6"/>
@@ -6907,22 +6907,22 @@
     </row>
     <row r="173" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A173" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B173" s="12">
         <v>44055</v>
       </c>
       <c r="C173" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D173" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D173" s="6" t="s">
+      <c r="E173" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E173" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="F173" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G173" s="6"/>
       <c r="H173" s="6"/>
@@ -6937,22 +6937,22 @@
     </row>
     <row r="174" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A174" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B174" s="12">
         <v>44055</v>
       </c>
       <c r="C174" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D174" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D174" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="E174" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F174" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G174" s="6"/>
       <c r="H174" s="6"/>
@@ -6967,22 +6967,22 @@
     </row>
     <row r="175" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A175" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B175" s="12">
         <v>44055</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D175" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E175" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F175" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G175" s="6"/>
       <c r="H175" s="6"/>
@@ -6997,22 +6997,22 @@
     </row>
     <row r="176" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A176" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B176" s="12">
         <v>44055</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D176" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E176" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F176" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G176" s="6"/>
       <c r="H176" s="6"/>
@@ -7027,22 +7027,22 @@
     </row>
     <row r="177" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A177" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B177" s="12">
         <v>44055</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D177" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E177" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F177" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G177" s="6"/>
       <c r="H177" s="6"/>
@@ -7057,22 +7057,22 @@
     </row>
     <row r="178" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A178" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B178" s="12">
         <v>44055</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D178" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E178" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F178" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G178" s="6"/>
       <c r="H178" s="6"/>
@@ -7087,22 +7087,22 @@
     </row>
     <row r="179" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A179" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B179" s="12">
         <v>44055</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D179" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E179" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F179" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G179" s="6"/>
       <c r="H179" s="6"/>
@@ -7117,22 +7117,22 @@
     </row>
     <row r="180" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A180" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B180" s="12">
         <v>44055</v>
       </c>
       <c r="C180" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D180" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E180" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F180" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G180" s="6"/>
       <c r="H180" s="6"/>
@@ -7147,22 +7147,22 @@
     </row>
     <row r="181" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A181" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B181" s="12">
         <v>44055</v>
       </c>
       <c r="C181" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D181" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E181" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F181" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G181" s="6"/>
       <c r="H181" s="6"/>
@@ -7177,22 +7177,22 @@
     </row>
     <row r="182" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A182" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B182" s="12">
         <v>44055</v>
       </c>
       <c r="C182" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D182" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E182" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F182" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G182" s="6"/>
       <c r="H182" s="6"/>
@@ -7207,22 +7207,22 @@
     </row>
     <row r="183" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A183" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B183" s="12">
         <v>44055</v>
       </c>
       <c r="C183" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D183" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E183" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F183" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G183" s="6"/>
       <c r="H183" s="6"/>
@@ -7237,22 +7237,22 @@
     </row>
     <row r="184" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A184" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B184" s="12">
         <v>44055</v>
       </c>
       <c r="C184" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D184" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E184" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F184" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G184" s="6"/>
       <c r="H184" s="6"/>
@@ -7267,22 +7267,22 @@
     </row>
     <row r="185" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A185" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B185" s="12">
         <v>44055</v>
       </c>
       <c r="C185" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D185" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E185" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F185" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G185" s="6"/>
       <c r="H185" s="6"/>
@@ -7297,22 +7297,22 @@
     </row>
     <row r="186" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A186" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B186" s="12">
         <v>44055</v>
       </c>
       <c r="C186" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D186" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E186" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F186" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G186" s="6"/>
       <c r="H186" s="6"/>
@@ -7327,22 +7327,22 @@
     </row>
     <row r="187" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A187" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B187" s="12">
         <v>44055</v>
       </c>
       <c r="C187" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D187" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E187" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F187" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G187" s="6"/>
       <c r="H187" s="6"/>
@@ -7357,22 +7357,22 @@
     </row>
     <row r="188" spans="1:16" ht="13" x14ac:dyDescent="0.15">
       <c r="A188" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B188" s="12">
         <v>44055</v>
       </c>
       <c r="C188" s="6" t="s">
-        <v>47</v>
+        <v>162</v>
       </c>
       <c r="D188" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E188" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F188" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G188" s="6"/>
       <c r="H188" s="6"/>
@@ -22068,7 +22068,7 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -22076,7 +22076,7 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>